<commit_message>
trying to pull american made companies
</commit_message>
<xml_diff>
--- a/data_retrieval/scraping/scraping_tools/usa_companies.xlsx
+++ b/data_retrieval/scraping/scraping_tools/usa_companies.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27629"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15940" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13960" windowHeight="16040" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="114">
   <si>
     <t>Company Name</t>
   </si>
@@ -30,9 +30,6 @@
     <t>All American Clothing</t>
   </si>
   <si>
-    <t>All USA Clothing</t>
-  </si>
-  <si>
     <t>American Apparel</t>
   </si>
   <si>
@@ -90,9 +87,6 @@
     <t>Left Field</t>
   </si>
   <si>
-    <t>Loggerhead Apparel</t>
-  </si>
-  <si>
     <t>Michael Stars</t>
   </si>
   <si>
@@ -132,30 +126,18 @@
     <t>Wild Fox</t>
   </si>
   <si>
-    <t>All American jeans</t>
-  </si>
-  <si>
     <t>Baldwin Denim</t>
   </si>
   <si>
-    <t>Bullet Blues designer jeans</t>
-  </si>
-  <si>
     <t>True Religion</t>
   </si>
   <si>
-    <t>Shoes &amp; footwear</t>
-  </si>
-  <si>
     <t>Alden</t>
   </si>
   <si>
     <t>Allen Edmonds</t>
   </si>
   <si>
-    <t>Body and Sole Comfort: Insoles</t>
-  </si>
-  <si>
     <t>Capps Shoe Company</t>
   </si>
   <si>
@@ -168,9 +150,6 @@
     <t>Munro Shoes</t>
   </si>
   <si>
-    <t>Oakstreet Bootmakers</t>
-  </si>
-  <si>
     <t>Quoddy</t>
   </si>
   <si>
@@ -198,9 +177,6 @@
     <t>Tom's of Maine</t>
   </si>
   <si>
-    <t>Furniture, cookware and home</t>
-  </si>
-  <si>
     <t>360 Cookware</t>
   </si>
   <si>
@@ -333,18 +309,12 @@
     <t>Wren &amp; Cooper</t>
   </si>
   <si>
-    <t>Electronics</t>
-  </si>
-  <si>
     <t>Channellock</t>
   </si>
   <si>
     <t>Stihl</t>
   </si>
   <si>
-    <t>Airstream: Campers</t>
-  </si>
-  <si>
     <t>Annin Flagmakers</t>
   </si>
   <si>
@@ -379,6 +349,18 @@
   </si>
   <si>
     <t>SportPort</t>
+  </si>
+  <si>
+    <t>12091233011</t>
+  </si>
+  <si>
+    <t>Bullet Blues</t>
+  </si>
+  <si>
+    <t>Loggerhead Tools</t>
+  </si>
+  <si>
+    <t>Wolverine</t>
   </si>
 </sst>
 </file>
@@ -427,8 +409,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -439,13 +427,19 @@
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="13">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -775,10 +769,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B121"/>
+  <dimension ref="A1:B113"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
+      <selection activeCell="B113" sqref="A1:B113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -797,611 +791,742 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>68</v>
       </c>
       <c r="B2">
-        <v>9359772011</v>
+        <v>7203411011</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>52</v>
+      </c>
+      <c r="B3">
+        <v>13737084011</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>37</v>
+      </c>
+      <c r="B4">
+        <v>2581917011</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>2</v>
+      </c>
+      <c r="B5">
+        <v>9359772011</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>38</v>
+      </c>
+      <c r="B6">
+        <v>2581967011</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>3</v>
+      </c>
+      <c r="B7">
+        <v>2582091011</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>98</v>
+      </c>
+      <c r="B10">
+        <v>3017071011</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>11</v>
+        <v>35</v>
+      </c>
+      <c r="B11">
+        <v>14028585011</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>12</v>
+        <v>69</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
-        <v>13</v>
+        <v>6</v>
+      </c>
+      <c r="B13">
+        <v>5370930011</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>14</v>
+        <v>64</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="s">
-        <v>15</v>
+        <v>71</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1">
+        <v>111</v>
+      </c>
+      <c r="B18">
+        <v>7674244011</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
       <c r="A19" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
       <c r="A20" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
       <c r="A21" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1">
+        <v>39</v>
+      </c>
+      <c r="B21">
+        <v>7728549011</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
       <c r="A22" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1">
+        <v>96</v>
+      </c>
+      <c r="B22">
+        <v>2587064011</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
       <c r="A23" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
       <c r="A24" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
       <c r="A25" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
       <c r="A26" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1">
+        <v>53</v>
+      </c>
+      <c r="B26">
+        <v>5350534011</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
       <c r="A27" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
       <c r="A28" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
       <c r="A29" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1">
+        <v>11</v>
+      </c>
+      <c r="B29">
+        <v>7648096011</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
       <c r="A30" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1">
+        <v>99</v>
+      </c>
+      <c r="B30">
+        <v>2591892011</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
       <c r="A31" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1">
+        <v>12</v>
+      </c>
+      <c r="B31">
+        <v>8435832011</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
       <c r="A32" t="s">
-        <v>31</v>
+        <v>76</v>
       </c>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" t="s">
-        <v>32</v>
+        <v>13</v>
+      </c>
+      <c r="B33">
+        <v>11736847011</v>
       </c>
     </row>
     <row r="34" spans="1:2">
       <c r="A34" t="s">
-        <v>33</v>
+        <v>100</v>
       </c>
     </row>
     <row r="35" spans="1:2">
       <c r="A35" t="s">
-        <v>34</v>
+        <v>14</v>
       </c>
     </row>
     <row r="36" spans="1:2">
       <c r="A36" t="s">
-        <v>35</v>
+        <v>15</v>
       </c>
     </row>
     <row r="37" spans="1:2">
       <c r="A37" t="s">
-        <v>36</v>
+        <v>16</v>
       </c>
       <c r="B37">
-        <v>3050453011</v>
+        <v>2593225011</v>
       </c>
     </row>
     <row r="38" spans="1:2">
       <c r="A38" t="s">
-        <v>37</v>
+        <v>77</v>
       </c>
     </row>
     <row r="39" spans="1:2">
       <c r="A39" t="s">
-        <v>38</v>
+        <v>17</v>
+      </c>
+      <c r="B39">
+        <v>5371106011</v>
       </c>
     </row>
     <row r="40" spans="1:2">
       <c r="A40" t="s">
-        <v>39</v>
+        <v>65</v>
       </c>
     </row>
     <row r="41" spans="1:2">
       <c r="A41" t="s">
-        <v>29</v>
+        <v>18</v>
+      </c>
+      <c r="B41">
+        <v>5371119011</v>
       </c>
     </row>
     <row r="42" spans="1:2">
       <c r="A42" t="s">
-        <v>32</v>
+        <v>54</v>
+      </c>
+      <c r="B42">
+        <v>8932879011</v>
       </c>
     </row>
     <row r="43" spans="1:2">
       <c r="A43" t="s">
-        <v>40</v>
+        <v>55</v>
+      </c>
+      <c r="B43">
+        <v>2593871011</v>
       </c>
     </row>
     <row r="44" spans="1:2">
       <c r="A44" t="s">
-        <v>41</v>
+        <v>19</v>
       </c>
     </row>
     <row r="45" spans="1:2">
       <c r="A45" t="s">
-        <v>42</v>
+        <v>67</v>
       </c>
     </row>
     <row r="46" spans="1:2">
       <c r="A46" t="s">
-        <v>43</v>
+        <v>20</v>
+      </c>
+      <c r="B46">
+        <v>2594636011</v>
       </c>
     </row>
     <row r="47" spans="1:2">
       <c r="A47" t="s">
-        <v>44</v>
+        <v>101</v>
+      </c>
+      <c r="B47">
+        <v>15229973011</v>
       </c>
     </row>
     <row r="48" spans="1:2">
       <c r="A48" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2">
       <c r="A49" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="50" spans="1:1">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2">
       <c r="A50" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="51" spans="1:1">
+        <v>56</v>
+      </c>
+      <c r="B50">
+        <v>14576217011</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2">
       <c r="A51" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="52" spans="1:1">
+        <v>57</v>
+      </c>
+      <c r="B51">
+        <v>2595663011</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2">
       <c r="A52" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="53" spans="1:1">
+        <v>112</v>
+      </c>
+      <c r="B52">
+        <v>2595670011</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2">
       <c r="A53" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="54" spans="1:1">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2">
       <c r="A54" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="55" spans="1:1">
+        <v>41</v>
+      </c>
+      <c r="B54">
+        <v>3034181011</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2">
       <c r="A55" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="56" spans="1:1">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2">
       <c r="A56" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="57" spans="1:1">
+        <v>104</v>
+      </c>
+      <c r="B56" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2">
       <c r="A57" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="58" spans="1:1">
+        <v>22</v>
+      </c>
+      <c r="B57">
+        <v>2596511011</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2">
       <c r="A58" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="59" spans="1:1">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2">
       <c r="A59" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="60" spans="1:1">
+        <v>42</v>
+      </c>
+      <c r="B59">
+        <v>3036205011</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2">
       <c r="A60" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="61" spans="1:1">
+        <v>59</v>
+      </c>
+      <c r="B60">
+        <v>9494120011</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2">
       <c r="A61" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="62" spans="1:1">
+        <v>23</v>
+      </c>
+      <c r="B61">
+        <v>3036388011</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2">
       <c r="A62" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="63" spans="1:1">
+        <v>105</v>
+      </c>
+      <c r="B62">
+        <v>8126460011</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2">
       <c r="A63" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="64" spans="1:1">
+      <c r="B63">
+        <v>2597461011</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2">
       <c r="A64" t="s">
+        <v>113</v>
+      </c>
+      <c r="B64">
+        <v>2530792011</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2">
+      <c r="A65" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2">
+      <c r="A66" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2">
+      <c r="A67" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="65" spans="1:1">
-      <c r="A65" t="s">
+    <row r="68" spans="1:2">
+      <c r="A68" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2">
+      <c r="A69" t="s">
+        <v>26</v>
+      </c>
+      <c r="B69">
+        <v>7481324011</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2">
+      <c r="A70" t="s">
+        <v>43</v>
+      </c>
+      <c r="B70">
+        <v>2600273011</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2">
+      <c r="A71" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2">
+      <c r="A72" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2">
+      <c r="A73" t="s">
+        <v>45</v>
+      </c>
+      <c r="B73">
+        <v>2599474011</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2">
+      <c r="A74" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2">
+      <c r="A75" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2">
+      <c r="A76" t="s">
+        <v>47</v>
+      </c>
+      <c r="B76">
+        <v>15861306011</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2">
+      <c r="A77" t="s">
+        <v>28</v>
+      </c>
+      <c r="B77">
+        <v>8319999011</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2">
+      <c r="A78" t="s">
+        <v>81</v>
+      </c>
+      <c r="B78">
+        <v>11875001011</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2">
+      <c r="A79" t="s">
+        <v>83</v>
+      </c>
+      <c r="B79">
+        <v>2600587011</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2">
+      <c r="A80" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="66" spans="1:1">
-      <c r="A66" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="67" spans="1:1">
-      <c r="A67" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="68" spans="1:1">
-      <c r="A68" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="69" spans="1:1">
-      <c r="A69" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="70" spans="1:1">
-      <c r="A70" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="71" spans="1:1">
-      <c r="A71" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="72" spans="1:1">
-      <c r="A72" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="73" spans="1:1">
-      <c r="A73" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="74" spans="1:1">
-      <c r="A74" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="75" spans="1:1">
-      <c r="A75" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="76" spans="1:1">
-      <c r="A76" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="77" spans="1:1">
-      <c r="A77" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="78" spans="1:1">
-      <c r="A78" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="79" spans="1:1">
-      <c r="A79" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="80" spans="1:1">
-      <c r="A80" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="81" spans="1:1">
+      <c r="B80">
+        <v>2600587011</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2">
       <c r="A81" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="82" spans="1:1">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2">
       <c r="A82" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="83" spans="1:1">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2">
       <c r="A83" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="84" spans="1:1">
+        <v>109</v>
+      </c>
+      <c r="B83">
+        <v>15768724011</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2">
       <c r="A84" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="85" spans="1:1">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2">
       <c r="A85" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="86" spans="1:1">
+        <v>107</v>
+      </c>
+      <c r="B85">
+        <v>6459934011</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2">
       <c r="A86" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="87" spans="1:1">
+        <v>84</v>
+      </c>
+      <c r="B86">
+        <v>9114273011</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2">
       <c r="A87" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="88" spans="1:1">
+        <v>97</v>
+      </c>
+      <c r="B87">
+        <v>3043693011</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2">
       <c r="A88" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="89" spans="1:1">
+    <row r="89" spans="1:2">
       <c r="A89" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2">
+      <c r="A90" t="s">
+        <v>49</v>
+      </c>
+      <c r="B90">
+        <v>8913129011</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2">
+      <c r="A91" t="s">
+        <v>40</v>
+      </c>
+      <c r="B91">
+        <v>2592259011</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2">
+      <c r="A92" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2">
+      <c r="A93" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="90" spans="1:1">
-      <c r="A90" t="s">
+    <row r="94" spans="1:2">
+      <c r="A94" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2">
+      <c r="A95" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2">
+      <c r="A96" t="s">
+        <v>51</v>
+      </c>
+      <c r="B96">
+        <v>2602440011</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2">
+      <c r="A97" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="91" spans="1:1">
-      <c r="A91" t="s">
+    <row r="98" spans="1:2">
+      <c r="A98" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="92" spans="1:1">
-      <c r="A92" t="s">
+    <row r="99" spans="1:2">
+      <c r="A99" t="s">
+        <v>36</v>
+      </c>
+      <c r="B99">
+        <v>2602737011</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2">
+      <c r="A100" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2">
+      <c r="A101" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="93" spans="1:1">
-      <c r="A93" t="s">
+    <row r="102" spans="1:2">
+      <c r="A102" t="s">
+        <v>108</v>
+      </c>
+      <c r="B102">
+        <v>9418296011</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2">
+      <c r="A103" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="94" spans="1:1">
-      <c r="A94" t="s">
+      <c r="B103">
+        <v>9623314011</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2">
+      <c r="A104" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="95" spans="1:1">
-      <c r="A95" t="s">
+    <row r="105" spans="1:2">
+      <c r="A105" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="96" spans="1:1">
-      <c r="A96" t="s">
+      <c r="B105">
+        <v>12081674011</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2">
+      <c r="A106" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2">
+      <c r="A107" t="s">
+        <v>63</v>
+      </c>
+      <c r="B107">
+        <v>11149562011</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2">
+      <c r="A108" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2">
+      <c r="A109" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2">
+      <c r="A110" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="97" spans="1:1">
-      <c r="A97" t="s">
+      <c r="B110">
+        <v>8999942011</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2">
+      <c r="A111" t="s">
+        <v>34</v>
+      </c>
+      <c r="B111">
+        <v>3050453011</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2">
+      <c r="A112" t="s">
         <v>94</v>
-      </c>
-    </row>
-    <row r="98" spans="1:1">
-      <c r="A98" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="99" spans="1:1">
-      <c r="A99" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="100" spans="1:1">
-      <c r="A100" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="101" spans="1:1">
-      <c r="A101" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="102" spans="1:1">
-      <c r="A102" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="103" spans="1:1">
-      <c r="A103" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="104" spans="1:1">
-      <c r="A104" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="105" spans="1:1">
-      <c r="A105" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="106" spans="1:1">
-      <c r="A106" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="107" spans="1:1">
-      <c r="A107" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="108" spans="1:1">
-      <c r="A108" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="109" spans="1:1">
-      <c r="A109" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="110" spans="1:1">
-      <c r="A110" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="111" spans="1:1">
-      <c r="A111" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="112" spans="1:1">
-      <c r="A112" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="113" spans="1:1">
       <c r="A113" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="114" spans="1:1">
-      <c r="A114" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="115" spans="1:1">
-      <c r="A115" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="116" spans="1:1">
-      <c r="A116" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="117" spans="1:1">
-      <c r="A117" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="118" spans="1:1">
-      <c r="A118" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="119" spans="1:1">
-      <c r="A119" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="120" spans="1:1">
-      <c r="A120" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="121" spans="1:1">
-      <c r="A121" t="s">
-        <v>118</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="A2:B121">
+    <sortCondition ref="A2"/>
+  </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>

</xml_diff>